<commit_message>
Fix bug, Update and Change some Logic in Back-end
</commit_message>
<xml_diff>
--- a/server/excels/Book1.xlsx
+++ b/server/excels/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4Code\ONETEST\onetest\server\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52535936-950A-4A4D-B6C2-54B6447AC5E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E60BD5-0F02-4995-950A-8CFF303E4A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9072" xr2:uid="{7551E280-3FDD-44B7-9C6F-47B4F100C063}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{7551E280-3FDD-44B7-9C6F-47B4F100C063}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="29">
   <si>
     <t>Tên</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>31/10/2015</t>
-  </si>
-  <si>
-    <t>31/10/2016</t>
   </si>
   <si>
     <t>31/10/2017</t>
@@ -486,7 +483,7 @@
   <dimension ref="B2:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -494,20 +491,21 @@
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
@@ -521,7 +519,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
@@ -535,7 +533,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
@@ -549,7 +547,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
@@ -563,7 +561,7 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
@@ -577,7 +575,7 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
@@ -591,7 +589,7 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
@@ -605,7 +603,7 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
@@ -619,7 +617,7 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
@@ -633,7 +631,7 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
@@ -647,7 +645,7 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
@@ -661,7 +659,7 @@
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
@@ -675,7 +673,7 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
@@ -685,11 +683,8 @@
       <c r="C15" t="s">
         <v>1</v>
       </c>
-      <c r="D15" t="s">
-        <v>14</v>
-      </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
@@ -700,10 +695,10 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
@@ -714,10 +709,10 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
@@ -728,10 +723,10 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
@@ -742,10 +737,10 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
@@ -756,10 +751,10 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
@@ -770,10 +765,10 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
@@ -784,10 +779,10 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
@@ -798,10 +793,10 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
@@ -812,10 +807,10 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
@@ -826,10 +821,10 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
@@ -840,10 +835,10 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>